<commit_message>
Update 13-12-2024 and 12-12-2024
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siser\Documents\Authence\Timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60F78B1-3180-4942-9C09-CC61E0CC7893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73F29DC-16A2-4DCA-B86D-8A875A8AD538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -439,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:K30"/>
+  <dimension ref="D2:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,6 +1206,66 @@
         <v>31</v>
       </c>
     </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>29</v>
+      </c>
+      <c r="E31" s="1">
+        <v>45638</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>30</v>
+      </c>
+      <c r="E32" s="1">
+        <v>45639</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <v>31</v>
+      </c>
+      <c r="E33" s="1">
+        <v>45640</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>